<commit_message>
Corrección de datos - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_006.xlsx
+++ b/ControlCambios/02_Evaluacion_Desarrollador/Rechazadas/EvalDes_006.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\02_Evaluacion_Desarrollador\Rechazadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AF643F-EFBC-42B6-A43A-C28C8BBDD1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE9ADB7-D5BC-45F5-8DDD-44DA8504B549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,21 +43,12 @@
     <t>Nombre:</t>
   </si>
   <si>
-    <t>Nicolás Barcia Quintela</t>
-  </si>
-  <si>
     <t>Correo:</t>
   </si>
   <si>
-    <t>nicolas.barcia@rai.usc.es</t>
-  </si>
-  <si>
     <t>ID Empleado:</t>
   </si>
   <si>
-    <t>NBQ_050100</t>
-  </si>
-  <si>
     <t>Evaluación</t>
   </si>
   <si>
@@ -95,6 +86,15 @@
   </si>
   <si>
     <t>1/1</t>
+  </si>
+  <si>
+    <t>Jesús Campos Manjón</t>
+  </si>
+  <si>
+    <t>jesus.campos@rai.usc.es</t>
+  </si>
+  <si>
+    <t>JMC_180902</t>
   </si>
 </sst>
 </file>
@@ -597,6 +597,126 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -612,133 +732,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1050,7 +1050,7 @@
   <dimension ref="C1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:I13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,24 +1083,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25" t="s">
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="62"/>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1108,45 +1108,45 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="30" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1161,10 +1161,10 @@
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="29"/>
+      <c r="C11" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="62"/>
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1173,17 +1173,17 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="70"/>
+      <c r="C13" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1191,167 +1191,167 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
+      <c r="C15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="12"/>
-      <c r="D16" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
+      <c r="D16" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="48"/>
     </row>
     <row r="17" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="12"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="59"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
     </row>
     <row r="18" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="63"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="12"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
+      <c r="C20" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="3:16" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="12"/>
-      <c r="D21" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="67"/>
+      <c r="D21" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="12"/>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
+      <c r="C23" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="3:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="12"/>
-      <c r="D24" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
+      <c r="D24" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
     </row>
     <row r="25" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="12"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="47"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="40"/>
     </row>
     <row r="26" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="12"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="44"/>
     </row>
     <row r="27" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="12"/>
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
+      <c r="C28" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="12"/>
-      <c r="D29" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="55"/>
+      <c r="D29" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="48"/>
       <c r="P29" s="18"/>
     </row>
     <row r="30" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="12"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="59"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="12"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="59"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="12"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="63"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="56"/>
     </row>
     <row r="33" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="19"/>
@@ -1364,21 +1364,36 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="38"/>
+      <c r="C34" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="D16:J18"/>
+    <mergeCell ref="C20:E20"/>
     <mergeCell ref="C34:H34"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="D21:J21"/>
@@ -1386,21 +1401,6 @@
     <mergeCell ref="D24:J26"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="D29:J32"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="D16:J18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{D29749FD-0B3A-4CF2-8B86-44A587644656}"/>

</xml_diff>